<commit_message>
adicionando imagens e pequenas alteracoes na planilha
</commit_message>
<xml_diff>
--- a/ornito_inform.xlsx
+++ b/ornito_inform.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f93d456693b9d57a/Documentos/Estudos/Excel/ornitoinformes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f93d456693b9d57a/Documentos/Estudos/Excel/ornitoinform/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="194" documentId="8_{220182B4-DFAB-4E59-AAF2-4E042440A98C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A34BE8A5-C87A-4115-A8B6-38540C166E43}"/>
+  <xr:revisionPtr revIDLastSave="195" documentId="8_{220182B4-DFAB-4E59-AAF2-4E042440A98C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{23495855-2BAE-4F1A-BAB3-B169590AEF39}"/>
   <bookViews>
-    <workbookView xWindow="9075" yWindow="1875" windowWidth="13800" windowHeight="12435" xr2:uid="{8DD86D12-9F5F-4CE0-B19D-AFA87B02E160}"/>
+    <workbookView xWindow="4980" yWindow="1320" windowWidth="21600" windowHeight="13215" activeTab="1" xr2:uid="{8DD86D12-9F5F-4CE0-B19D-AFA87B02E160}"/>
   </bookViews>
   <sheets>
     <sheet name="TITULAR" sheetId="1" r:id="rId1"/>
@@ -77,9 +77,6 @@
     <t>CÔNJUGE</t>
   </si>
   <si>
-    <t>DEPENTENTE CÔNJUGE</t>
-  </si>
-  <si>
     <t>1. DADOS DO TÍTULAR</t>
   </si>
   <si>
@@ -303,6 +300,9 @@
   </si>
   <si>
     <t>info_CITI_2024.pdf</t>
+  </si>
+  <si>
+    <t>DEPENDENTE CÔNJUGE</t>
   </si>
 </sst>
 </file>
@@ -310,10 +310,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="169" formatCode="000&quot;.&quot;000&quot;.&quot;000&quot;-&quot;00"/>
-    <numFmt numFmtId="170" formatCode="&quot;(&quot;00&quot;)&quot;00000&quot;-&quot;0000"/>
-    <numFmt numFmtId="171" formatCode="00000\-000"/>
-    <numFmt numFmtId="172" formatCode="&quot;R$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="164" formatCode="000&quot;.&quot;000&quot;.&quot;000&quot;-&quot;00"/>
+    <numFmt numFmtId="165" formatCode="&quot;(&quot;00&quot;)&quot;00000&quot;-&quot;0000"/>
+    <numFmt numFmtId="166" formatCode="00000\-000"/>
+    <numFmt numFmtId="167" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -514,13 +514,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -539,16 +536,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -557,23 +554,25 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hiperlink" xfId="2" builtinId="8"/>
@@ -582,13 +581,13 @@
   </cellStyles>
   <dxfs count="4">
     <dxf>
-      <numFmt numFmtId="22" formatCode="mmm/yy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="&quot;R$&quot;\ #,##0.00"/>
+      <numFmt numFmtId="167" formatCode="&quot;R$&quot;\ #,##0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="22" formatCode="mmm/yy"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2590,9 +2589,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{98F7361E-4327-4E46-811F-A6C4B71BB494}" name="Tabela2" displayName="Tabela2" ref="C8:E28" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="C8:E28" xr:uid="{98F7361E-4327-4E46-811F-A6C4B71BB494}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{FBCA7E7C-FCF0-4511-8D0E-BBC15B6C44C3}" name="DATA" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{E618A9FA-FD66-4BD4-8EFB-807E3AB37B6A}" name="CATEGORIA" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{1BC17ABE-D9D0-4A3D-896F-DF5008B1C920}" name="VALOR" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{FBCA7E7C-FCF0-4511-8D0E-BBC15B6C44C3}" name="DATA" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{E618A9FA-FD66-4BD4-8EFB-807E3AB37B6A}" name="CATEGORIA" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{1BC17ABE-D9D0-4A3D-896F-DF5008B1C920}" name="VALOR" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2917,8 +2916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEEF39C0-06C2-40CB-943D-9A1DA1B06696}">
   <dimension ref="A3:E19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2929,120 +2928,120 @@
   <sheetData>
     <row r="3" spans="3:5" ht="19.5" x14ac:dyDescent="0.3">
       <c r="C3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="3:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+    </row>
+    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="11">
+        <v>65360892301</v>
+      </c>
+    </row>
+    <row r="9" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C9" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="7">
+        <v>37409</v>
+      </c>
+    </row>
+    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C10" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="6">
+        <v>121215478</v>
+      </c>
+    </row>
+    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C12" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="13">
+        <v>65320987</v>
+      </c>
+    </row>
+    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="12">
+        <v>19936254178</v>
+      </c>
+    </row>
+    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C15" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="12">
+        <v>19936254178</v>
+      </c>
+    </row>
+    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C16" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C7" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C8" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="12">
-        <v>65360892301</v>
-      </c>
-    </row>
-    <row r="9" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C9" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="8">
-        <v>37409</v>
-      </c>
-    </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C10" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="7">
-        <v>121215478</v>
-      </c>
-    </row>
-    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C11" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C12" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="7" t="s">
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C17" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C13" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="14">
-        <v>65320987</v>
-      </c>
-    </row>
-    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C14" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="13">
-        <v>19936254178</v>
-      </c>
-    </row>
-    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C15" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="13">
-        <v>19936254178</v>
-      </c>
-    </row>
-    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C16" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C17" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C18" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>19</v>
+      <c r="C18" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="11" t="s">
-        <v>19</v>
+      <c r="D19" s="10" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -3067,8 +3066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4A31794-0426-4044-B236-A45D64DDD154}">
   <dimension ref="A3:E22"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3079,122 +3078,122 @@
   <sheetData>
     <row r="3" spans="3:5" ht="19.5" x14ac:dyDescent="0.3">
       <c r="C3" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="3:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="C4" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
     </row>
     <row r="6" spans="3:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C6" s="20" t="s">
-        <v>24</v>
+      <c r="C6" s="17" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="3:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C7" s="19">
+      <c r="C7" s="23">
         <f>SUM(D11,D16,D21)</f>
         <v>17020000</v>
       </c>
-      <c r="D7" s="18"/>
+      <c r="D7" s="24"/>
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="15"/>
+    </row>
+    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="14">
+        <v>5000000</v>
+      </c>
+    </row>
+    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C14" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="16"/>
-    </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C10" s="4" t="s">
+      <c r="D14" s="15"/>
+    </row>
+    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C16" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C11" s="4" t="s">
+      <c r="D16" s="14">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C17" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="15">
-        <v>5000000</v>
-      </c>
-    </row>
-    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C12" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="5" t="s">
+      <c r="D17" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C14" s="17" t="s">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C19" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="16"/>
-    </row>
-    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C15" s="4" t="s">
+      <c r="D19" s="15"/>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C20" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C21" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C16" s="4" t="s">
+      <c r="D21" s="14">
+        <v>12000000</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C22" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="15">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C17" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17" s="5" t="s">
+      <c r="D22" s="4" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C19" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="D19" s="16"/>
-    </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C20" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C21" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D21" s="15">
-        <v>12000000</v>
-      </c>
-    </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C22" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -3235,141 +3234,141 @@
   <sheetData>
     <row r="3" spans="3:5" ht="19.5" x14ac:dyDescent="0.3">
       <c r="C3" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="3:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="C4" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
     </row>
     <row r="5" spans="3:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="3:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="3:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
+      <c r="C7" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="E8" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="22" t="s">
-        <v>33</v>
-      </c>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C9" s="25">
+      <c r="C9" s="21">
         <v>45822</v>
       </c>
-      <c r="D9" s="23"/>
-      <c r="E9" s="24">
+      <c r="D9" s="19"/>
+      <c r="E9" s="20">
         <v>3000</v>
       </c>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C10" s="25"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="24"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="20"/>
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C11" s="25"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="24"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="20"/>
     </row>
     <row r="12" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C12" s="25"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="24"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="20"/>
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C13" s="25"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="24"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="20"/>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C14" s="25"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="24"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="20"/>
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C15" s="25"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="24"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="20"/>
     </row>
     <row r="16" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C16" s="25"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="24"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="20"/>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C17" s="25"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="24"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="20"/>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C18" s="25"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="24"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="20"/>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C19" s="25"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="24"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="20"/>
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C20" s="25"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="24"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="20"/>
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C21" s="25"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="24"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="20"/>
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C22" s="25"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="24"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="20"/>
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C23" s="25"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="24"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="20"/>
     </row>
     <row r="24" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C24" s="25"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="24"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="20"/>
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C25" s="25"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="24"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="20"/>
     </row>
     <row r="26" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C26" s="25"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="24"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="20"/>
     </row>
     <row r="27" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C27" s="25"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="24"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="20"/>
     </row>
     <row r="28" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C28" s="25"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="24"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3400,253 +3399,253 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="26" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="26" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="26" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="26" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="26" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="26" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="26" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="26" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="26" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="26" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="26" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="26" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="26" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="26" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="26" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="26" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="26" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="26" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="26" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="26" t="s">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="26" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="26" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="26" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="26" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="26" t="s">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="26" t="s">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="26" t="s">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="26" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="26" t="s">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="26" t="s">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="26" t="s">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="26" t="s">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="26" t="s">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="26" t="s">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="26" t="s">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="26" t="s">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="26" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="26" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="26" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>